<commit_message>
createNewFileHandler (App.tsx)を削除. strageControlHandler にマージ
</commit_message>
<xml_diff>
--- a/doc/Development_Spec.xlsx
+++ b/doc/Development_Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KOTA/work/TsuriMapMaker/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF148D-C97C-BC4C-BE8C-29EDE4D736E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0ACDFA-29D5-1B4C-B71B-361D0F602E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="11" xr2:uid="{2C8663B7-A646-664E-AD48-D017962260BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="11" xr2:uid="{2C8663B7-A646-664E-AD48-D017962260BA}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="179">
   <si>
     <t>Tsuri Map Maker</t>
     <phoneticPr fontId="1"/>
@@ -1571,6 +1571,78 @@
     <rPh sb="6" eb="10">
       <t xml:space="preserve">シンキサクセイ </t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Next State</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>State ID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S1|S2|S3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>asEditMode
+(boolean)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>asViewMode
+(boolean)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mapEditorIsOpen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>asInitMode
+(boolean)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Window Type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mode</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>storageControl
+IsOpen</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1798,7 +1870,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1910,6 +1982,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1980,7 +2061,47 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -11696,8 +11817,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5205684" y="1358899"/>
-          <a:ext cx="1225374" cy="863256"/>
+          <a:off x="5222754" y="1622458"/>
+          <a:ext cx="1228788" cy="877458"/>
           <a:chOff x="3739697" y="615795"/>
           <a:chExt cx="1221454" cy="871700"/>
         </a:xfrm>
@@ -11721,6 +11842,9 @@
           <a:prstGeom prst="roundRect">
             <a:avLst/>
           </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
@@ -12507,8 +12631,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2653672" y="3465426"/>
-          <a:ext cx="1638457" cy="882001"/>
+          <a:off x="2660500" y="3764491"/>
+          <a:ext cx="1645285" cy="896203"/>
           <a:chOff x="3739697" y="772163"/>
           <a:chExt cx="1221454" cy="715332"/>
         </a:xfrm>
@@ -13256,8 +13380,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4735062" y="3353271"/>
-          <a:ext cx="1520864" cy="1119481"/>
+          <a:off x="4748718" y="3648785"/>
+          <a:ext cx="1527692" cy="1137234"/>
           <a:chOff x="3739697" y="772163"/>
           <a:chExt cx="1221454" cy="715332"/>
         </a:xfrm>
@@ -14021,8 +14145,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6910525" y="3353271"/>
-          <a:ext cx="1524784" cy="1119481"/>
+          <a:off x="6934423" y="3648785"/>
+          <a:ext cx="1528198" cy="1137234"/>
           <a:chOff x="3739697" y="772163"/>
           <a:chExt cx="1221454" cy="715332"/>
         </a:xfrm>
@@ -14786,8 +14910,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2742572" y="5563037"/>
-          <a:ext cx="1642376" cy="876744"/>
+          <a:off x="2749400" y="5894056"/>
+          <a:ext cx="1649204" cy="890947"/>
           <a:chOff x="3739697" y="772163"/>
           <a:chExt cx="1221454" cy="715332"/>
         </a:xfrm>
@@ -15535,8 +15659,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4587051" y="7318748"/>
-          <a:ext cx="1634537" cy="882002"/>
+          <a:off x="4600707" y="7674621"/>
+          <a:ext cx="1641365" cy="896204"/>
           <a:chOff x="3739697" y="772163"/>
           <a:chExt cx="1221454" cy="715332"/>
         </a:xfrm>
@@ -16284,8 +16408,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6419624" y="5560122"/>
-          <a:ext cx="1638457" cy="872832"/>
+          <a:off x="6440108" y="5891141"/>
+          <a:ext cx="1645285" cy="887035"/>
           <a:chOff x="3739697" y="772163"/>
           <a:chExt cx="1221454" cy="715332"/>
         </a:xfrm>
@@ -18995,13 +19119,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
+      <xdr:colOff>508000</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>187556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>785514</xdr:colOff>
+      <xdr:colOff>797702</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>219507</xdr:rowOff>
     </xdr:to>
@@ -19018,8 +19142,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6222999" y="1330556"/>
-          <a:ext cx="3135015" cy="6661351"/>
+          <a:off x="6223000" y="1584556"/>
+          <a:ext cx="3147202" cy="6661351"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -19108,6 +19232,18 @@
             <a:gd name="connsiteY4" fmla="*/ 3085 h 6839134"/>
             <a:gd name="connsiteX5" fmla="*/ 254414 w 4016411"/>
             <a:gd name="connsiteY5" fmla="*/ 329543 h 6839134"/>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 4032024"/>
+            <a:gd name="connsiteY0" fmla="*/ 6839134 h 6839134"/>
+            <a:gd name="connsiteX1" fmla="*/ 3435180 w 4032024"/>
+            <a:gd name="connsiteY1" fmla="*/ 6179810 h 6839134"/>
+            <a:gd name="connsiteX2" fmla="*/ 4013827 w 4032024"/>
+            <a:gd name="connsiteY2" fmla="*/ 2605801 h 6839134"/>
+            <a:gd name="connsiteX3" fmla="*/ 3228570 w 4032024"/>
+            <a:gd name="connsiteY3" fmla="*/ 473455 h 6839134"/>
+            <a:gd name="connsiteX4" fmla="*/ 1879059 w 4032024"/>
+            <a:gd name="connsiteY4" fmla="*/ 3085 h 6839134"/>
+            <a:gd name="connsiteX5" fmla="*/ 254414 w 4032024"/>
+            <a:gd name="connsiteY5" fmla="*/ 329543 h 6839134"/>
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst>
@@ -19132,22 +19268,22 @@
           </a:cxnLst>
           <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
-            <a:path w="4016411" h="6839134">
+            <a:path w="4032024" h="6839134">
               <a:moveTo>
                 <a:pt x="0" y="6839134"/>
               </a:moveTo>
               <a:cubicBezTo>
                 <a:pt x="1147181" y="6666665"/>
-                <a:pt x="2294362" y="6494196"/>
-                <a:pt x="2963333" y="5788641"/>
+                <a:pt x="2766209" y="6885365"/>
+                <a:pt x="3435180" y="6179810"/>
               </a:cubicBezTo>
               <a:cubicBezTo>
-                <a:pt x="3632304" y="5083086"/>
-                <a:pt x="3969621" y="3491665"/>
+                <a:pt x="4104151" y="5474255"/>
+                <a:pt x="4048262" y="3556860"/>
                 <a:pt x="4013827" y="2605801"/>
               </a:cubicBezTo>
               <a:cubicBezTo>
-                <a:pt x="4058033" y="1719937"/>
+                <a:pt x="3979392" y="1654742"/>
                 <a:pt x="3524448" y="734772"/>
                 <a:pt x="3228570" y="473455"/>
               </a:cubicBezTo>
@@ -19634,7 +19770,7 @@
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="2:4" ht="19" customHeight="1">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -19645,7 +19781,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="19" customHeight="1">
-      <c r="B10" s="38"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="4" t="s">
         <v>75</v>
       </c>
@@ -19654,7 +19790,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" ht="19" customHeight="1">
-      <c r="B11" s="38"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="4" t="s">
         <v>76</v>
       </c>
@@ -19684,7 +19820,7 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -19695,7 +19831,7 @@
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="40"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -19705,11 +19841,11 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="6"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="42" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -19720,7 +19856,7 @@
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="42"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="7" t="s">
         <v>77</v>
       </c>
@@ -19729,7 +19865,7 @@
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="42"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="7" t="s">
         <v>78</v>
       </c>
@@ -19738,7 +19874,7 @@
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="40"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="7" t="s">
         <v>79</v>
       </c>
@@ -19748,8 +19884,8 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="6"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="6" t="s">
@@ -19763,52 +19899,52 @@
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
     </row>
     <row r="25" spans="2:4">
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
     </row>
     <row r="26" spans="2:4">
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
     </row>
     <row r="29" spans="2:4">
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
     </row>
     <row r="30" spans="2:4">
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
     </row>
     <row r="31" spans="2:4">
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
     </row>
     <row r="32" spans="2:4">
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
     </row>
     <row r="33" spans="3:4">
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
     </row>
     <row r="34" spans="3:4">
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
     </row>
     <row r="35" spans="3:4">
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -19832,7 +19968,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:B15 B17:B18 B22:B1048576">
-    <cfRule type="expression" dxfId="31" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19887,15 +20023,226 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2948B-CB17-CC43-978A-D5EB3695E688}">
-  <dimension ref="A1"/>
+  <dimension ref="L4:R12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="93" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
-  <sheetData/>
+  <cols>
+    <col min="12" max="12" width="9.42578125" style="32" customWidth="1"/>
+    <col min="13" max="14" width="16.85546875" style="32" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="32" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="32" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="32" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="12:18">
+      <c r="M4" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+    </row>
+    <row r="5" spans="12:18" ht="38">
+      <c r="L5" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="N5" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="O5" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="P5" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q5" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="R5" s="37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="12:18">
+      <c r="L6" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="M6" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" s="37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="12:18">
+      <c r="L7" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="M7" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" s="37"/>
+    </row>
+    <row r="8" spans="12:18">
+      <c r="L8" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="M8" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="37"/>
+    </row>
+    <row r="9" spans="12:18">
+      <c r="L9" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="M9" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" s="37"/>
+    </row>
+    <row r="10" spans="12:18">
+      <c r="L10" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="M10" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="37"/>
+    </row>
+    <row r="11" spans="12:18">
+      <c r="L11" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="M11" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" s="37"/>
+    </row>
+    <row r="12" spans="12:18">
+      <c r="L12" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="M12" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="R12" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="O6:Q12">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:N12">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M6:M12">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -19909,7 +20256,7 @@
       <pane xSplit="12" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -19942,30 +20289,30 @@
       <c r="C2" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="45"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="31"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="49"/>
+      <c r="I2" s="52"/>
       <c r="J2" s="31"/>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="46" t="s">
+      <c r="L2" s="52"/>
+      <c r="M2" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="51" t="s">
+      <c r="N2" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="46" t="s">
+      <c r="O2" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="P2" s="47" t="s">
+      <c r="P2" s="50" t="s">
         <v>46</v>
       </c>
     </row>
@@ -19990,10 +20337,10 @@
       <c r="L3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="47"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="50"/>
     </row>
     <row r="4" spans="1:16" ht="35" customHeight="1">
       <c r="C4" s="33">
@@ -21109,112 +21456,112 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="D34:W1011 D4:W11 D5:D12 G12:H12 J11:K12 D31:W32 D31:D33 G31:H33 J31:K33 D28:F29 D21:W28 D14:W19">
-    <cfRule type="expression" dxfId="30" priority="9">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>D4=D3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:P1048576">
-    <cfRule type="expression" dxfId="29" priority="25">
+    <cfRule type="expression" dxfId="33" priority="25">
       <formula>COUNTA($E4:$K4)&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:L21 L22:L33 E22:E33">
-    <cfRule type="expression" dxfId="28" priority="27">
+    <cfRule type="expression" dxfId="32" priority="27">
       <formula>E21=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32 J32:K32 G26:G28 J26:K28">
-    <cfRule type="expression" dxfId="27" priority="29">
+    <cfRule type="expression" dxfId="31" priority="29">
       <formula>G26=G24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:L9 G29 J29:K29 J16:J19 G16:G19">
-    <cfRule type="expression" dxfId="26" priority="30">
+    <cfRule type="expression" dxfId="30" priority="30">
       <formula>F8=F5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:W12 F8:L11 K13:K14 D29:W29 G22:G23 H22:H24 J16:J19 J22:J23 G16:G19">
-    <cfRule type="expression" dxfId="25" priority="32">
+    <cfRule type="expression" dxfId="29" priority="32">
       <formula>D8=D6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:Q1012">
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>$C4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:XFD112">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>$B4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:I11">
-    <cfRule type="expression" dxfId="22" priority="54">
+    <cfRule type="expression" dxfId="26" priority="54">
       <formula>I10=I6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:L12 I10:I11 G23:G24 H24:H25 J23:J24 D13:W13 D33:W33 K16:K19 K23:K28">
-    <cfRule type="expression" dxfId="21" priority="73">
+    <cfRule type="expression" dxfId="25" priority="73">
       <formula>D10=D7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:XFD111">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$A4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12 K29 D30:W30 D20:W20">
-    <cfRule type="expression" dxfId="19" priority="79">
+    <cfRule type="expression" dxfId="23" priority="79">
       <formula>D12=D8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I14 H20:H22 G20 J20">
-    <cfRule type="expression" dxfId="18" priority="88">
+    <cfRule type="expression" dxfId="22" priority="88">
       <formula>G13=G7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:L15 G30:G31 J30:K31 J20:K20 G20">
-    <cfRule type="expression" dxfId="17" priority="92">
+    <cfRule type="expression" dxfId="21" priority="92">
       <formula>F15=F10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13 G20:H21 J20:J21">
-    <cfRule type="expression" dxfId="16" priority="94">
+    <cfRule type="expression" dxfId="20" priority="94">
       <formula>G13=G8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="15" priority="103">
+    <cfRule type="expression" dxfId="19" priority="103">
       <formula>I12=I7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="14" priority="107">
+    <cfRule type="expression" dxfId="18" priority="107">
       <formula>I14=I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 G13:H13 J13:K13">
-    <cfRule type="expression" dxfId="13" priority="109">
+    <cfRule type="expression" dxfId="17" priority="109">
       <formula>D13=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="expression" dxfId="12" priority="126">
+    <cfRule type="expression" dxfId="16" priority="126">
       <formula>K15=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:W33 K32">
-    <cfRule type="expression" dxfId="11" priority="133">
+    <cfRule type="expression" dxfId="15" priority="133">
       <formula>D32=D25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33 J33:K33">
-    <cfRule type="expression" dxfId="10" priority="147">
+    <cfRule type="expression" dxfId="14" priority="147">
       <formula>G33=G26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:K32 K20:K22">
-    <cfRule type="expression" dxfId="9" priority="149">
+    <cfRule type="expression" dxfId="13" priority="149">
       <formula>K20=K14</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21243,12 +21590,12 @@
   <sheetData>
     <row r="1" spans="1:59" ht="33">
       <c r="A1" s="11"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="59"/>
       <c r="H1" s="14">
         <f>H3</f>
         <v>44636</v>
@@ -21459,18 +21806,18 @@
       </c>
     </row>
     <row r="2" spans="1:59" ht="19" thickBot="1">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="53" t="s">
+      <c r="C2" s="61"/>
+      <c r="D2" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="53"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="19">
         <f>H3</f>
         <v>44636</v>
@@ -22260,45 +22607,45 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H1:BG1">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>YEAR(H1)=YEAR(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:BG2">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>MONTH(H2)=MONTH(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:BG27">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>AND($B4&lt;&gt;"", B$3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C1048576">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>$B4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BG35">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>AND(H$3&gt;=$D4, H$3&lt;=$E4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:BG3">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>H1 = TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:BG1 A2:B2 D2:BG2 A3:BG1048576">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>OR(A1="n/a", A1="-")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:XFD1048576">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>AND(H$3&gt;=$F4, H$3&lt;=$G4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>AND($G4&lt;&gt;"", H$3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>